<commit_message>
Removed coordinate data from Configuration file. Coordinates and other data for formatting outputs now are in a table loaded in the script
</commit_message>
<xml_diff>
--- a/01_Configuration/SCANClim_Configuration.xlsx
+++ b/01_Configuration/SCANClim_Configuration.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://efsa815-my.sharepoint.com/personal/andrea_maiorano_efsa_europa_eu/Documents/03_PLH/Projects/SCANClim/01_Configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{874B1FA3-8351-44C2-A6E9-E9441DD188ED}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{55CF932C-CBE2-4039-AC3A-970B3C2C25EB}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32724" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
     <sheet name="Authors" sheetId="9" r:id="rId2"/>
     <sheet name="Pest_list" sheetId="1" r:id="rId3"/>
     <sheet name="Pest_status_to_be_included" sheetId="2" r:id="rId4"/>
-    <sheet name="Other settings" sheetId="4" r:id="rId5"/>
-    <sheet name="Climates_to_be_removed" sheetId="8" r:id="rId6"/>
-    <sheet name="tech" sheetId="6" r:id="rId7"/>
+    <sheet name="Climates_to_be_removed" sheetId="8" r:id="rId5"/>
+    <sheet name="Other settings" sheetId="4" r:id="rId6"/>
+    <sheet name="tech" sheetId="6" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="eu.nuts">tech!$N$2:$N$4</definedName>
-    <definedName name="fao.gaul">tech!$O$2:$O$4</definedName>
+    <definedName name="eu.nuts">tech!#REF!</definedName>
+    <definedName name="fao.gaul">tech!$D$2:$D$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Present, no details</t>
   </si>
@@ -99,127 +99,106 @@
     <t>List of pest status (according to EPPO) to be included in the analysis</t>
   </si>
   <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Recalculate EU27 Climate list</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>Climates</t>
+  </si>
+  <si>
+    <t>Dsb</t>
+  </si>
+  <si>
+    <t>Dsc</t>
+  </si>
+  <si>
+    <t>Download EPPO host table</t>
+  </si>
+  <si>
+    <t>Host_status_to_be_included</t>
+  </si>
+  <si>
+    <t>Climates_to_be_removed</t>
+  </si>
+  <si>
+    <t>tech</t>
+  </si>
+  <si>
+    <t>List of host status (according to EPPO) to be included in the analysis</t>
+  </si>
+  <si>
+    <t>List of additional climates to be removed from mapping. These are climates removed in addition from the climates not present in EU (removed or included in "Other settings" sheet).</t>
+  </si>
+  <si>
+    <t>Sheet needed for technical purposes. Do not modify</t>
+  </si>
+  <si>
+    <t>61b2d7f23653e1f2e9815f14ef7bfd80</t>
+  </si>
+  <si>
+    <t>Andrea Maiorano</t>
+  </si>
+  <si>
+    <t>Caterina Campese</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Select Region to map</t>
+  </si>
+  <si>
+    <t>EPPO API token</t>
+  </si>
+  <si>
+    <t>Xylella fastidiosa</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Caribbean</t>
+  </si>
+  <si>
     <t>Europe</t>
   </si>
   <si>
-    <t>Asia</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>America</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>no</t>
+    <t>Oceania</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Asia_SE</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>China_SE</t>
   </si>
   <si>
     <t>Region</t>
-  </si>
-  <si>
-    <t>x1</t>
-  </si>
-  <si>
-    <t>x2</t>
-  </si>
-  <si>
-    <t>y1</t>
-  </si>
-  <si>
-    <t>y2</t>
-  </si>
-  <si>
-    <t>xat</t>
-  </si>
-  <si>
-    <t>yat</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Caribbean</t>
-  </si>
-  <si>
-    <t>Oceania</t>
-  </si>
-  <si>
-    <t>Recalculate EU27 Climate list</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Ocean</t>
-  </si>
-  <si>
-    <t>Climates</t>
-  </si>
-  <si>
-    <t>Dsb</t>
-  </si>
-  <si>
-    <t>Dsc</t>
-  </si>
-  <si>
-    <t>eu.nuts</t>
-  </si>
-  <si>
-    <t>Download EPPO host table</t>
-  </si>
-  <si>
-    <t>Peru</t>
-  </si>
-  <si>
-    <t>Host_status_to_be_included</t>
-  </si>
-  <si>
-    <t>Climates_to_be_removed</t>
-  </si>
-  <si>
-    <t>tech</t>
-  </si>
-  <si>
-    <t>List of host status (according to EPPO) to be included in the analysis</t>
-  </si>
-  <si>
-    <t>List of additional climates to be removed from mapping. These are climates removed in addition from the climates not present in EU (removed or included in "Other settings" sheet).</t>
-  </si>
-  <si>
-    <t>Sheet needed for technical purposes. Do not modify</t>
-  </si>
-  <si>
-    <t>61b2d7f23653e1f2e9815f14ef7bfd80</t>
-  </si>
-  <si>
-    <t>Andrea Maiorano</t>
-  </si>
-  <si>
-    <t>Caterina Campese</t>
-  </si>
-  <si>
-    <t>Authors</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>China_SE</t>
-  </si>
-  <si>
-    <t>Asia_SE</t>
-  </si>
-  <si>
-    <t>Select Region to map</t>
-  </si>
-  <si>
-    <t>EPPO API token</t>
-  </si>
-  <si>
-    <t>Leucinodes pseudorbonalis</t>
   </si>
 </sst>
 </file>
@@ -725,10 +704,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -741,18 +720,18 @@
     </row>
     <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -779,17 +758,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -802,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -820,7 +799,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -875,99 +854,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="26.86328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climates not in EU" prompt="Select yes to exclude climates that are not in Europe from visualization" xr:uid="{67D655F5-1EE8-45C1-BEA6-D66676F22775}">
-          <x14:formula1>
-            <xm:f>tech!$L$2:$L$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry!" error="Please select a Region from the list" promptTitle="Regions" prompt="Please select a Region from the list" xr:uid="{00000000-0002-0000-0400-000000000000}">
-          <x14:formula1>
-            <xm:f>tech!$A$2:$A$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{482D41D3-29EE-49D4-85AA-B3E82588417B}">
-          <x14:formula1>
-            <xm:f>tech!$L$2:$L$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4:B5</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B4FD27-DD83-404E-B71B-70883D41A962}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -982,22 +868,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1005,344 +891,189 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climates not in EU" prompt="Select &quot;yes&quot; to exclude climates that are not in Europe from final output_x000a_" xr:uid="{67D655F5-1EE8-45C1-BEA6-D66676F22775}">
+          <x14:formula1>
+            <xm:f>tech!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{482D41D3-29EE-49D4-85AA-B3E82588417B}">
+          <x14:formula1>
+            <xm:f>tech!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4:B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry!" error="Please select a Region from the list" promptTitle="Region to plot" prompt="Select a Region from the list" xr:uid="{00000000-0002-0000-0400-000000000000}">
+          <x14:formula1>
+            <xm:f>tech!$A$2:$A$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.53125" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.53125" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2">
-        <v>-180</v>
-      </c>
-      <c r="C2">
-        <v>180</v>
-      </c>
-      <c r="D2">
-        <v>-60</v>
-      </c>
-      <c r="E2">
-        <v>90</v>
-      </c>
-      <c r="F2">
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>-180</v>
-      </c>
-      <c r="C3">
-        <v>-20</v>
-      </c>
-      <c r="D3">
-        <v>-60</v>
-      </c>
-      <c r="E3">
-        <v>90</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>180</v>
-      </c>
-      <c r="D4">
-        <v>-25</v>
-      </c>
-      <c r="E4">
-        <v>90</v>
-      </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>80</v>
-      </c>
-      <c r="C5">
-        <v>180</v>
-      </c>
-      <c r="D5">
-        <v>-50</v>
-      </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>-90</v>
-      </c>
-      <c r="C6">
-        <v>-70</v>
-      </c>
-      <c r="D6">
-        <v>15</v>
-      </c>
-      <c r="E6">
-        <v>25</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>-25</v>
-      </c>
-      <c r="C7">
-        <v>35</v>
-      </c>
-      <c r="D7">
-        <v>30</v>
-      </c>
-      <c r="E7">
-        <v>73</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8">
-        <v>110</v>
-      </c>
-      <c r="C8">
-        <v>180</v>
-      </c>
-      <c r="D8">
-        <v>-55</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9">
-        <v>-130</v>
-      </c>
-      <c r="C9">
-        <v>-50</v>
-      </c>
-      <c r="D9">
-        <v>20</v>
-      </c>
-      <c r="E9">
-        <v>65</v>
-      </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10">
-        <v>-85</v>
-      </c>
-      <c r="C10">
-        <v>-65</v>
-      </c>
-      <c r="D10">
-        <v>-20</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11">
-        <v>90</v>
-      </c>
-      <c r="C11">
-        <v>160</v>
-      </c>
-      <c r="D11">
-        <v>-25</v>
-      </c>
-      <c r="E11">
-        <v>35</v>
-      </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12">
-        <v>70</v>
-      </c>
-      <c r="C12">
-        <v>140</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>55</v>
-      </c>
-      <c r="F12">
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13">
-        <v>70</v>
-      </c>
-      <c r="C13">
-        <v>130</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>40</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G9">
-    <sortCondition ref="A1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A13">
+    <sortCondition ref="A3:A13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>